<commit_message>
Update Uurrooster.xlsx schedule file
The Uurrooster.xlsx file has been updated. Changes may include modifications to the schedule or timetable data.
</commit_message>
<xml_diff>
--- a/Uurrooster.xlsx
+++ b/Uurrooster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LUCA-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8577C62A-EDB5-46A6-BC3F-4D46D71B843B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40E9C65-8959-4BFB-8BDD-267D4614A960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{28AF1FA9-2C6A-4F87-8A25-50C42A1BDAE6}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" firstSheet="15" activeTab="18" xr2:uid="{28AF1FA9-2C6A-4F87-8A25-50C42A1BDAE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="93">
   <si>
     <t>Vakken</t>
   </si>
@@ -204,10 +204,157 @@
     <t>Agenda leeg</t>
   </si>
   <si>
-    <t>Agenda leeg vanaf hier en volgende maanden</t>
+    <t>Met theo naar coole winkel gaan in antwerpen?</t>
   </si>
   <si>
-    <t>Met theo naar coole winkel gaan in antwerpen?</t>
+    <t>Opdracht #1 - DAP</t>
+  </si>
+  <si>
+    <t>Briefing opdracht #1 - GOALS!</t>
+  </si>
+  <si>
+    <t>Wio - Thomas</t>
+  </si>
+  <si>
+    <t>Wio - Kilian</t>
+  </si>
+  <si>
+    <t>Wio</t>
+  </si>
+  <si>
+    <t>Rush GT</t>
+  </si>
+  <si>
+    <t>9U - Hocus Focus</t>
+  </si>
+  <si>
+    <t>In progress expo</t>
+  </si>
+  <si>
+    <t>9u - hocus focus</t>
+  </si>
+  <si>
+    <t>Wio - Thomas - Kilian</t>
+  </si>
+  <si>
+    <t>Wonder</t>
+  </si>
+  <si>
+    <t>Afspraak 10U in Kortrijk</t>
+  </si>
+  <si>
+    <t>Opdracht #2 - RenAIssance</t>
+  </si>
+  <si>
+    <t>Speeddate - Feedback</t>
+  </si>
+  <si>
+    <t>10u: briefing opdracht #2</t>
+  </si>
+  <si>
+    <t>Deadline opdracht #1</t>
+  </si>
+  <si>
+    <t>Intensieve werkweek / geen atelier</t>
+  </si>
+  <si>
+    <t>10U: briefing opdracht</t>
+  </si>
+  <si>
+    <t>Presentaties</t>
+  </si>
+  <si>
+    <t>Deadline eiwit shift</t>
+  </si>
+  <si>
+    <t>Projectweek eiwit shift</t>
+  </si>
+  <si>
+    <t>Geen les</t>
+  </si>
+  <si>
+    <t>Studio Digital: Hack the future</t>
+  </si>
+  <si>
+    <t>Pitch @ MSK</t>
+  </si>
+  <si>
+    <t>9U: Hokus Focus</t>
+  </si>
+  <si>
+    <t>Wio  - Kilian</t>
+  </si>
+  <si>
+    <t>9U: hokus focus</t>
+  </si>
+  <si>
+    <t>Studio Digital: opbouw + museumnacht (wio - thomas - kilian)</t>
+  </si>
+  <si>
+    <t>Afbraak</t>
+  </si>
+  <si>
+    <t>Studio Digital: Deadline opdracht #2</t>
+  </si>
+  <si>
+    <t>10U: feedback opdracht #3</t>
+  </si>
+  <si>
+    <t>Briefing opdracht #3: FUTURE OF THE InTerwebZ</t>
+  </si>
+  <si>
+    <t>Kerstvakantie</t>
+  </si>
+  <si>
+    <t>Deadline Opdracht #3</t>
+  </si>
+  <si>
+    <t>Einde semester 1!</t>
+  </si>
+  <si>
+    <t>Paasmaandag (digitaal kalender is mss fout)</t>
+  </si>
+  <si>
+    <t>Studiereis (briefing Toledo)</t>
+  </si>
+  <si>
+    <t>Kilian</t>
+  </si>
+  <si>
+    <t>Geen les + opstellen OCD + er is al les op zat!</t>
+  </si>
+  <si>
+    <t>Opencampusdag - AANWEZIG!</t>
+  </si>
+  <si>
+    <t>Opencampusdag</t>
+  </si>
+  <si>
+    <t>TBC - Bezoek aan expo New Technical Art Award</t>
+  </si>
+  <si>
+    <t>Deadline indienen internationale opdracht - 23U</t>
+  </si>
+  <si>
+    <t>Hemelvaart? (als het hemelvaart is, geen les)</t>
+  </si>
+  <si>
+    <t>Als het pinksteren is, geen les</t>
+  </si>
+  <si>
+    <t>Proefjury</t>
+  </si>
+  <si>
+    <t>Deadline indienen bachelorproef op Toledo - 23U</t>
+  </si>
+  <si>
+    <t>JURY</t>
+  </si>
+  <si>
+    <t>Opbouw graduation show</t>
+  </si>
+  <si>
+    <t>Graduation show</t>
   </si>
 </sst>
 </file>
@@ -378,7 +525,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -445,6 +592,11 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
@@ -1322,7 +1474,7 @@
   <dimension ref="B2:R48"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="D20" sqref="D18:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1962,7 +2114,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2098,17 +2250,25 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="40" t="s">
+        <v>67</v>
+      </c>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="40" t="s">
+        <v>68</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="D11" s="29"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="40" t="s">
+        <v>48</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
@@ -2214,7 +2374,9 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20" s="29"/>
       <c r="G20" s="3"/>
@@ -2504,7 +2666,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2640,17 +2802,25 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="40" t="s">
+        <v>46</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="40" t="s">
+        <v>69</v>
+      </c>
       <c r="D11" s="29"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="40" t="s">
+        <v>48</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
@@ -2762,7 +2932,9 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="D20" s="28" t="s">
         <v>3</v>
       </c>
@@ -3062,7 +3234,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3198,17 +3370,25 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="40" t="s">
+        <v>71</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="40" t="s">
+        <v>67</v>
+      </c>
       <c r="D11" s="29"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="40" t="s">
+        <v>46</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
@@ -3314,7 +3494,9 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20" s="29"/>
       <c r="G20" s="3"/>
@@ -3419,22 +3601,26 @@
         <v>45998</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
+      <c r="F30" s="39" t="s">
+        <v>70</v>
+      </c>
       <c r="G30" s="33"/>
       <c r="H30" s="33"/>
       <c r="I30" s="33"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="33"/>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
+      <c r="F31" s="39" t="s">
+        <v>72</v>
+      </c>
       <c r="G31" s="33"/>
       <c r="H31" s="33"/>
       <c r="I31" s="33"/>
@@ -3604,7 +3790,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3740,17 +3926,25 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="40" t="s">
+        <v>46</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="40" t="s">
+        <v>73</v>
+      </c>
       <c r="D11" s="29"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="40" t="s">
+        <v>48</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
@@ -3862,7 +4056,9 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="D20" s="28" t="s">
         <v>3</v>
       </c>
@@ -3977,9 +4173,11 @@
         <v>46005</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
+      <c r="C30" s="39" t="s">
+        <v>74</v>
+      </c>
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
       <c r="F30" s="33"/>
@@ -4162,7 +4360,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4298,17 +4496,25 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="40" t="s">
+        <v>46</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="40" t="s">
+        <v>67</v>
+      </c>
       <c r="D11" s="29"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="40" t="s">
+        <v>48</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
@@ -4414,7 +4620,9 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20" s="29"/>
       <c r="G20" s="3"/>
@@ -4704,7 +4912,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4810,29 +5018,11 @@
       <c r="B8" s="16">
         <v>0.375</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="15"/>
-      <c r="C9" s="4">
-        <v>204</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4">
-        <v>204</v>
-      </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
     </row>
@@ -4840,17 +5030,11 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="29"/>
-      <c r="G11" s="3"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
@@ -4858,29 +5042,11 @@
       <c r="B12" s="16">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="3"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="15"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="12">
-        <v>115</v>
-      </c>
-      <c r="F13" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" s="3"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
     </row>
@@ -4888,21 +5054,11 @@
       <c r="B14" s="16">
         <v>0.5</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="3"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="3"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
     </row>
@@ -4910,13 +5066,11 @@
       <c r="B16" s="16">
         <v>0.54166666666666663</v>
       </c>
-      <c r="F16" s="29"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
-      <c r="F17" s="29"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
     </row>
@@ -4924,37 +5078,11 @@
       <c r="B18" s="16">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
-      <c r="C19" s="4">
-        <v>204</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="4">
-        <v>309</v>
-      </c>
-      <c r="F19" s="29"/>
-      <c r="G19" s="4">
-        <v>204</v>
-      </c>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
     </row>
@@ -4962,21 +5090,11 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="3"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="3"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
     </row>
@@ -4984,25 +5102,11 @@
       <c r="B22" s="16">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="29"/>
-      <c r="G22" s="3"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="29"/>
-      <c r="G23" s="3"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
     </row>
@@ -5010,21 +5114,11 @@
       <c r="B24" s="16">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="3"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="15"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="3"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
     </row>
@@ -5076,19 +5170,19 @@
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
       <c r="C30" s="39" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="D30" s="39" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="E30" s="39" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="F30" s="39" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="G30" s="39" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="H30" s="33"/>
       <c r="I30" s="33"/>
@@ -5268,7 +5362,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5374,29 +5468,11 @@
       <c r="B8" s="16">
         <v>0.375</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="15"/>
-      <c r="C9" s="4">
-        <v>204</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4">
-        <v>204</v>
-      </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
     </row>
@@ -5404,17 +5480,11 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="29"/>
-      <c r="G11" s="3"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
@@ -5422,29 +5492,11 @@
       <c r="B12" s="16">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="3"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="15"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="12">
-        <v>115</v>
-      </c>
-      <c r="F13" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" s="3"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
     </row>
@@ -5452,21 +5504,11 @@
       <c r="B14" s="16">
         <v>0.5</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="3"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="3"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
     </row>
@@ -5474,13 +5516,11 @@
       <c r="B16" s="16">
         <v>0.54166666666666663</v>
       </c>
-      <c r="F16" s="29"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
-      <c r="F17" s="29"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
     </row>
@@ -5488,37 +5528,11 @@
       <c r="B18" s="16">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
-      <c r="C19" s="4">
-        <v>204</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="4">
-        <v>309</v>
-      </c>
-      <c r="F19" s="29"/>
-      <c r="G19" s="4">
-        <v>204</v>
-      </c>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
     </row>
@@ -5526,21 +5540,11 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="3"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="3"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
     </row>
@@ -5548,25 +5552,11 @@
       <c r="B22" s="16">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="29"/>
-      <c r="G22" s="3"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="29"/>
-      <c r="G23" s="3"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
     </row>
@@ -5574,21 +5564,11 @@
       <c r="B24" s="16">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="3"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="15"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="3"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
     </row>
@@ -5637,22 +5617,22 @@
         <v>46026</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
       <c r="C30" s="39" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="D30" s="39" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="E30" s="39" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="F30" s="39" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="G30" s="39" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="H30" s="33"/>
       <c r="I30" s="33"/>
@@ -5832,7 +5812,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5968,17 +5948,25 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="40" t="s">
+        <v>46</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="40" t="s">
+        <v>67</v>
+      </c>
       <c r="D11" s="29"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="40" t="s">
+        <v>48</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
@@ -6090,7 +6078,9 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="D20" s="29"/>
       <c r="E20" s="3"/>
       <c r="F20" s="29"/>
@@ -6388,7 +6378,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6524,15 +6514,21 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="40" t="s">
+        <v>46</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="40" t="s">
+        <v>67</v>
+      </c>
       <c r="D11" s="29"/>
       <c r="G11" s="3"/>
       <c r="H11" s="14"/>
@@ -6646,7 +6642,9 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="D20" s="29"/>
       <c r="E20" s="3"/>
       <c r="F20" s="29"/>
@@ -6763,7 +6761,9 @@
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
       <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
+      <c r="G30" s="39" t="s">
+        <v>76</v>
+      </c>
       <c r="H30" s="33"/>
       <c r="I30" s="33"/>
     </row>
@@ -6773,7 +6773,9 @@
       <c r="D31" s="33"/>
       <c r="E31" s="33"/>
       <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
+      <c r="G31" s="39" t="s">
+        <v>77</v>
+      </c>
       <c r="H31" s="33"/>
       <c r="I31" s="33"/>
     </row>
@@ -6941,8 +6943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F05623-E348-4555-8264-A129D987A943}">
   <dimension ref="B2:I46"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7313,8 +7315,12 @@
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
+      <c r="C30" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="39" t="s">
+        <v>90</v>
+      </c>
       <c r="E30" s="33"/>
       <c r="F30" s="33"/>
       <c r="G30" s="33"/>
@@ -7495,8 +7501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584AF639-35B2-4815-B4D2-171BB2FF563A}">
   <dimension ref="B2:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7632,7 +7638,9 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="40" t="s">
+        <v>43</v>
+      </c>
       <c r="D10" s="29"/>
       <c r="G10" s="3"/>
       <c r="H10" s="14"/>
@@ -7640,7 +7648,9 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="40" t="s">
+        <v>44</v>
+      </c>
       <c r="D11" s="29"/>
       <c r="G11" s="3"/>
       <c r="H11" s="14"/>
@@ -7650,7 +7660,9 @@
       <c r="B12" s="16">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="D12" s="29"/>
       <c r="E12" s="11" t="s">
         <v>5</v>
@@ -7742,12 +7754,16 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="D20" s="28" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="G20" s="40" t="s">
+        <v>46</v>
+      </c>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
     </row>
@@ -7867,7 +7883,7 @@
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
       <c r="F30" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G30" s="33"/>
       <c r="H30" s="33"/>
@@ -13598,7 +13614,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13734,17 +13750,25 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="40" t="s">
+        <v>46</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="40" t="s">
+        <v>49</v>
+      </c>
       <c r="D11" s="29"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="40" t="s">
+        <v>48</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
@@ -13850,7 +13874,9 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20" s="29"/>
       <c r="G20" s="3"/>
@@ -14140,7 +14166,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15248,7 +15274,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15617,10 +15643,14 @@
         <v>46138</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
+      <c r="C30" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="39" t="s">
+        <v>79</v>
+      </c>
       <c r="E30" s="33"/>
       <c r="F30" s="33"/>
       <c r="G30" s="33"/>
@@ -16356,7 +16386,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16471,7 +16501,9 @@
       <c r="G8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="14"/>
+      <c r="H8" s="42" t="s">
+        <v>83</v>
+      </c>
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
@@ -16492,9 +16524,13 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="40" t="s">
+        <v>80</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
@@ -16614,11 +16650,15 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="D20" s="29"/>
       <c r="E20" s="3"/>
       <c r="F20" s="29"/>
-      <c r="G20" s="3"/>
+      <c r="G20" s="40" t="s">
+        <v>81</v>
+      </c>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
     </row>
@@ -16732,7 +16772,9 @@
       <c r="E30" s="33"/>
       <c r="F30" s="33"/>
       <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
+      <c r="H30" s="39" t="s">
+        <v>82</v>
+      </c>
       <c r="I30" s="33"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
@@ -16910,7 +16952,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17046,9 +17088,13 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="40" t="s">
+        <v>80</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
@@ -17168,11 +17214,15 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="D20" s="29"/>
       <c r="E20" s="3"/>
       <c r="F20" s="29"/>
-      <c r="G20" s="3"/>
+      <c r="G20" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
     </row>
@@ -17182,7 +17232,9 @@
       <c r="D21" s="29"/>
       <c r="E21" s="3"/>
       <c r="F21" s="29"/>
-      <c r="G21" s="3"/>
+      <c r="G21" s="40" t="s">
+        <v>84</v>
+      </c>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
     </row>
@@ -17463,8 +17515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5749555B-B31D-4B8E-B8B7-3E108EEA2C9C}">
   <dimension ref="B2:I46"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+    <sheetView topLeftCell="B2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17600,9 +17652,13 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="40" t="s">
+        <v>80</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
@@ -17722,11 +17778,15 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="D20" s="29"/>
       <c r="E20" s="3"/>
       <c r="F20" s="29"/>
-      <c r="G20" s="3"/>
+      <c r="G20" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
     </row>
@@ -17833,7 +17893,7 @@
         <v>46166</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
@@ -17841,7 +17901,9 @@
       <c r="F30" s="33"/>
       <c r="G30" s="33"/>
       <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
+      <c r="I30" s="39" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="33"/>
@@ -18018,7 +18080,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18154,7 +18216,9 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="29"/>
       <c r="G10" s="3"/>
       <c r="H10" s="14"/>
@@ -18276,7 +18340,9 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="D20" s="29"/>
       <c r="E20" s="3"/>
       <c r="F20" s="29"/>
@@ -18387,13 +18453,15 @@
         <v>46173</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
       <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
+      <c r="G30" s="39" t="s">
+        <v>86</v>
+      </c>
       <c r="H30" s="33"/>
       <c r="I30" s="33"/>
     </row>
@@ -18572,7 +18640,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18708,9 +18776,13 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="40" t="s">
+        <v>80</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
@@ -18830,11 +18902,15 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="D20" s="29"/>
       <c r="E20" s="3"/>
       <c r="F20" s="29"/>
-      <c r="G20" s="3"/>
+      <c r="G20" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
     </row>
@@ -19125,8 +19201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{120B4AFD-6E8F-4856-8C19-5D1A19F22499}">
   <dimension ref="B2:I46"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19495,15 +19571,21 @@
         <v>46187</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
+      <c r="C30" s="39" t="s">
+        <v>87</v>
+      </c>
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
       <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
+      <c r="G30" s="39" t="s">
+        <v>88</v>
+      </c>
       <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
+      <c r="I30" s="39" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="33"/>
@@ -19680,7 +19762,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19816,17 +19898,25 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="40" t="s">
+        <v>46</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="40" t="s">
+        <v>51</v>
+      </c>
       <c r="D11" s="29"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="40" t="s">
+        <v>48</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
@@ -19938,7 +20028,9 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="D20" s="28" t="s">
         <v>3</v>
       </c>
@@ -19950,7 +20042,9 @@
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="40" t="s">
+        <v>50</v>
+      </c>
       <c r="D21" s="29" t="s">
         <v>4</v>
       </c>
@@ -20238,7 +20332,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20609,8 +20703,12 @@
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
+      <c r="C30" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="39" t="s">
+        <v>90</v>
+      </c>
       <c r="E30" s="33"/>
       <c r="F30" s="33"/>
       <c r="G30" s="33"/>
@@ -20791,8 +20889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F103211F-71C8-473B-B6C0-5C3DB387ED5E}">
   <dimension ref="B2:I46"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21163,13 +21261,27 @@
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
+      <c r="C30" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="G30" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="H30" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="I30" s="39" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="33"/>
@@ -21346,7 +21458,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21482,17 +21594,25 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="40" t="s">
+        <v>52</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="40" t="s">
+        <v>49</v>
+      </c>
       <c r="D11" s="29"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="40" t="s">
+        <v>53</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
@@ -21508,7 +21628,9 @@
       <c r="F12" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
     </row>
@@ -21604,7 +21726,9 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="D20" s="29"/>
       <c r="E20" s="3"/>
       <c r="F20" s="29"/>
@@ -21902,7 +22026,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22038,17 +22162,25 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="40" t="s">
+        <v>46</v>
+      </c>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="40" t="s">
+        <v>46</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="40" t="s">
+        <v>55</v>
+      </c>
       <c r="D11" s="29"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="40" t="s">
+        <v>56</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
@@ -22056,7 +22188,9 @@
       <c r="B12" s="16">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="40" t="s">
+        <v>57</v>
+      </c>
       <c r="D12" s="29"/>
       <c r="E12" s="11" t="s">
         <v>5</v>
@@ -22160,7 +22294,9 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="D20" s="7"/>
       <c r="E20" s="3"/>
       <c r="F20" s="29"/>
@@ -22273,7 +22409,9 @@
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
+      <c r="C30" s="39" t="s">
+        <v>58</v>
+      </c>
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
       <c r="F30" s="33"/>
@@ -22456,7 +22594,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="C18" sqref="C18:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22562,13 +22700,13 @@
       <c r="B8" s="16">
         <v>0.375</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="36" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="36" t="s">
         <v>6</v>
       </c>
       <c r="H8" s="14"/>
@@ -22576,13 +22714,13 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="15"/>
-      <c r="C9" s="4">
+      <c r="C9" s="41">
         <v>204</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="41">
         <v>204</v>
       </c>
       <c r="H9" s="14"/>
@@ -22592,17 +22730,17 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="37"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="29"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
@@ -22610,7 +22748,7 @@
       <c r="B12" s="16">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="29"/>
       <c r="E12" s="11" t="s">
         <v>5</v>
@@ -22618,13 +22756,13 @@
       <c r="F12" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="37"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="15"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="29"/>
       <c r="E13" s="12">
         <v>115</v>
@@ -22632,7 +22770,7 @@
       <c r="F13" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="37"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
     </row>
@@ -22640,21 +22778,21 @@
       <c r="B14" s="16">
         <v>0.5</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="29"/>
       <c r="E14" s="10"/>
       <c r="F14" s="29"/>
-      <c r="G14" s="3"/>
+      <c r="G14" s="37"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="29"/>
       <c r="E15" s="10"/>
       <c r="F15" s="29"/>
-      <c r="G15" s="3"/>
+      <c r="G15" s="37"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
     </row>
@@ -22676,7 +22814,7 @@
       <c r="B18" s="16">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="36" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="28" t="s">
@@ -22686,7 +22824,7 @@
         <v>7</v>
       </c>
       <c r="F18" s="29"/>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="36" t="s">
         <v>6</v>
       </c>
       <c r="H18" s="14"/>
@@ -22694,7 +22832,7 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
-      <c r="C19" s="4">
+      <c r="C19" s="41">
         <v>204</v>
       </c>
       <c r="D19" s="29" t="s">
@@ -22704,7 +22842,7 @@
         <v>309</v>
       </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="4">
+      <c r="G19" s="41">
         <v>204</v>
       </c>
       <c r="H19" s="14"/>
@@ -22714,21 +22852,21 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="29"/>
       <c r="E20" s="3"/>
       <c r="F20" s="29"/>
-      <c r="G20" s="3"/>
+      <c r="G20" s="37"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="29"/>
       <c r="E21" s="3"/>
       <c r="F21" s="29"/>
-      <c r="G21" s="3"/>
+      <c r="G21" s="37"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
     </row>
@@ -22736,25 +22874,25 @@
       <c r="B22" s="16">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C22" s="3"/>
+      <c r="C22" s="37"/>
       <c r="D22" s="29"/>
       <c r="E22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="29"/>
-      <c r="G22" s="3"/>
+      <c r="G22" s="37"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
-      <c r="C23" s="3"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="29"/>
       <c r="E23" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F23" s="29"/>
-      <c r="G23" s="3"/>
+      <c r="G23" s="37"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
     </row>
@@ -22762,21 +22900,21 @@
       <c r="B24" s="16">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C24" s="3"/>
+      <c r="C24" s="37"/>
       <c r="D24" s="29"/>
       <c r="E24" s="3"/>
       <c r="F24" s="29"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="37"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="15"/>
-      <c r="C25" s="3"/>
+      <c r="C25" s="37"/>
       <c r="D25" s="29"/>
       <c r="E25" s="3"/>
       <c r="F25" s="29"/>
-      <c r="G25" s="3"/>
+      <c r="G25" s="37"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
     </row>
@@ -22825,10 +22963,10 @@
         <v>45963</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
       <c r="C30" s="39" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="D30" s="39" t="s">
         <v>41</v>
@@ -22840,7 +22978,7 @@
         <v>41</v>
       </c>
       <c r="G30" s="39" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="H30" s="33"/>
       <c r="I30" s="33"/>
@@ -23020,7 +23158,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23126,13 +23264,13 @@
       <c r="B8" s="16">
         <v>0.375</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="36" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="36" t="s">
         <v>6</v>
       </c>
       <c r="H8" s="14"/>
@@ -23140,13 +23278,13 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="15"/>
-      <c r="C9" s="4">
+      <c r="C9" s="41">
         <v>204</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="41">
         <v>204</v>
       </c>
       <c r="H9" s="14"/>
@@ -23156,17 +23294,25 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="37" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="37" t="s">
+        <v>46</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="37" t="s">
+        <v>60</v>
+      </c>
       <c r="D11" s="29"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="37" t="s">
+        <v>61</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
@@ -23174,7 +23320,7 @@
       <c r="B12" s="16">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="29"/>
       <c r="E12" s="11" t="s">
         <v>5</v>
@@ -23182,13 +23328,13 @@
       <c r="F12" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="37"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="15"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="29"/>
       <c r="E13" s="12">
         <v>115</v>
@@ -23196,7 +23342,7 @@
       <c r="F13" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="37"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
     </row>
@@ -23204,21 +23350,21 @@
       <c r="B14" s="16">
         <v>0.5</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="29"/>
       <c r="E14" s="10"/>
       <c r="F14" s="29"/>
-      <c r="G14" s="3"/>
+      <c r="G14" s="37"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="29"/>
       <c r="E15" s="10"/>
       <c r="F15" s="29"/>
-      <c r="G15" s="3"/>
+      <c r="G15" s="37"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
     </row>
@@ -23240,14 +23386,14 @@
       <c r="B18" s="16">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="36" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="29"/>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="36" t="s">
         <v>6</v>
       </c>
       <c r="H18" s="14"/>
@@ -23255,14 +23401,14 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
-      <c r="C19" s="4">
+      <c r="C19" s="41">
         <v>204</v>
       </c>
       <c r="E19" s="4">
         <v>309</v>
       </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="4">
+      <c r="G19" s="41">
         <v>204</v>
       </c>
       <c r="H19" s="14"/>
@@ -23272,19 +23418,21 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="37" t="s">
+        <v>45</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20" s="29"/>
-      <c r="G20" s="3"/>
+      <c r="G20" s="37"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="37"/>
       <c r="E21" s="3"/>
       <c r="F21" s="29"/>
-      <c r="G21" s="3"/>
+      <c r="G21" s="37"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
     </row>
@@ -23292,23 +23440,23 @@
       <c r="B22" s="16">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C22" s="3"/>
+      <c r="C22" s="37"/>
       <c r="E22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="29"/>
-      <c r="G22" s="3"/>
+      <c r="G22" s="37"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
-      <c r="C23" s="3"/>
+      <c r="C23" s="37"/>
       <c r="E23" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F23" s="29"/>
-      <c r="G23" s="3"/>
+      <c r="G23" s="37"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
     </row>
@@ -23316,19 +23464,19 @@
       <c r="B24" s="16">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C24" s="3"/>
+      <c r="C24" s="37"/>
       <c r="E24" s="3"/>
       <c r="F24" s="29"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="37"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="15"/>
-      <c r="C25" s="3"/>
+      <c r="C25" s="37"/>
       <c r="E25" s="3"/>
       <c r="F25" s="29"/>
-      <c r="G25" s="3"/>
+      <c r="G25" s="37"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
     </row>
@@ -23379,11 +23527,15 @@
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
+      <c r="C30" s="39" t="s">
+        <v>63</v>
+      </c>
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
       <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
+      <c r="G30" s="39" t="s">
+        <v>62</v>
+      </c>
       <c r="H30" s="33"/>
       <c r="I30" s="33"/>
     </row>
@@ -23562,7 +23714,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G28"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23668,9 +23820,6 @@
       <c r="B8" s="16">
         <v>0.375</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="D8" s="28" t="s">
         <v>25</v>
       </c>
@@ -23682,9 +23831,6 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="15"/>
-      <c r="C9" s="4">
-        <v>204</v>
-      </c>
       <c r="D9" s="29" t="s">
         <v>1</v>
       </c>
@@ -23698,17 +23844,19 @@
       <c r="B10" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="3"/>
       <c r="D10" s="29"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
-      <c r="C11" s="3"/>
       <c r="D11" s="29"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="40" t="s">
+        <v>46</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
@@ -23716,7 +23864,6 @@
       <c r="B12" s="16">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C12" s="3"/>
       <c r="D12" s="29"/>
       <c r="E12" s="11" t="s">
         <v>5</v>
@@ -23730,7 +23877,6 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="15"/>
-      <c r="C13" s="3"/>
       <c r="D13" s="29"/>
       <c r="E13" s="12">
         <v>115</v>
@@ -23746,7 +23892,6 @@
       <c r="B14" s="16">
         <v>0.5</v>
       </c>
-      <c r="C14" s="3"/>
       <c r="D14" s="29"/>
       <c r="E14" s="10"/>
       <c r="F14" s="29"/>
@@ -23756,7 +23901,6 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
-      <c r="C15" s="3"/>
       <c r="D15" s="29"/>
       <c r="E15" s="10"/>
       <c r="F15" s="29"/>
@@ -23782,9 +23926,6 @@
       <c r="B18" s="16">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="D18" s="28" t="s">
         <v>26</v>
       </c>
@@ -23800,9 +23941,6 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
-      <c r="C19" s="4">
-        <v>204</v>
-      </c>
       <c r="D19" s="29" t="s">
         <v>1</v>
       </c>
@@ -23820,7 +23958,6 @@
       <c r="B20" s="16">
         <v>0.625</v>
       </c>
-      <c r="C20" s="3"/>
       <c r="D20" s="29"/>
       <c r="E20" s="3"/>
       <c r="F20" s="29"/>
@@ -23830,7 +23967,6 @@
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
-      <c r="C21" s="3"/>
       <c r="D21" s="29"/>
       <c r="E21" s="3"/>
       <c r="F21" s="29"/>
@@ -23842,7 +23978,6 @@
       <c r="B22" s="16">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C22" s="3"/>
       <c r="D22" s="29"/>
       <c r="E22" s="5" t="s">
         <v>9</v>
@@ -23854,7 +23989,6 @@
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
-      <c r="C23" s="3"/>
       <c r="D23" s="29"/>
       <c r="E23" s="6" t="s">
         <v>10</v>
@@ -23868,7 +24002,6 @@
       <c r="B24" s="16">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C24" s="3"/>
       <c r="D24" s="29"/>
       <c r="E24" s="3"/>
       <c r="F24" s="29"/>
@@ -23878,7 +24011,6 @@
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="15"/>
-      <c r="C25" s="3"/>
       <c r="D25" s="29"/>
       <c r="E25" s="3"/>
       <c r="F25" s="29"/>
@@ -23934,13 +24066,15 @@
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
       <c r="C30" s="39" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="D30" s="39" t="s">
         <v>41</v>
       </c>
       <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
+      <c r="F30" s="39" t="s">
+        <v>65</v>
+      </c>
       <c r="G30" s="33"/>
       <c r="H30" s="33"/>
       <c r="I30" s="33"/>

</xml_diff>

<commit_message>
Add Storytelling lesson and update schedule
Added the first lesson document for Storytelling and updated the schedule spreadsheet to reflect recent changes.
</commit_message>
<xml_diff>
--- a/Uurrooster.xlsx
+++ b/Uurrooster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sethv\Desktop\LUCA-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54547A27-0ED3-4E1B-81F4-E84CD84E6EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CF43DF-05E6-49EB-9C93-4C154BC9770A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="1" activeTab="1" xr2:uid="{28AF1FA9-2C6A-4F87-8A25-50C42A1BDAE6}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="117">
   <si>
     <t>Vakken</t>
   </si>
@@ -424,6 +424,9 @@
   </si>
   <si>
     <t>mss werken voor atelier ofzo al (storyboarding)</t>
+  </si>
+  <si>
+    <t>Hack the future inschrijven</t>
   </si>
 </sst>
 </file>
@@ -7580,7 +7583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584AF639-35B2-4815-B4D2-171BB2FF563A}">
   <dimension ref="B2:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -13702,7 +13705,7 @@
   <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14057,7 +14060,9 @@
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
+      <c r="C30" s="39" t="s">
+        <v>116</v>
+      </c>
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
       <c r="F30" s="33"/>

</xml_diff>